<commit_message>
1. Uzupełniona rekcja 2. Uzupełnione n-v verbindungen. 3. Uzupełniony wortschatz-w3
</commit_message>
<xml_diff>
--- a/_rektion/rektion-sätze.xlsx
+++ b/_rektion/rektion-sätze.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="504">
   <si>
     <t>Er ändert etwas an seinem Projekt.</t>
   </si>
@@ -1300,6 +1300,234 @@
   </si>
   <si>
     <t>Teraz trzeba się uzbroić w cierpliwość.</t>
+  </si>
+  <si>
+    <t>sich reißen um A</t>
+  </si>
+  <si>
+    <t>zabijać się o [coś] (pot.)</t>
+  </si>
+  <si>
+    <t>aus-gehen von D</t>
+  </si>
+  <si>
+    <t>pochodzić od [czegoś]/mieć swoje źródło w [czymś]</t>
+  </si>
+  <si>
+    <t>jdm erpressen mit D</t>
+  </si>
+  <si>
+    <t>szantażować kogoś [czymś]</t>
+  </si>
+  <si>
+    <t>heran-kommen an A</t>
+  </si>
+  <si>
+    <t>zbliżać się do [czegoś]</t>
+  </si>
+  <si>
+    <t>sich entsinnen an A</t>
+  </si>
+  <si>
+    <t>przypominać sobie [kogoś/coś]</t>
+  </si>
+  <si>
+    <t>jdn unterstützen bei D/in D</t>
+  </si>
+  <si>
+    <t>pomagać komuś przy [czymś]/w [czymś]</t>
+  </si>
+  <si>
+    <t>neigen zu D</t>
+  </si>
+  <si>
+    <t>mieć tendencję do [czegoś]</t>
+  </si>
+  <si>
+    <t>zurück-gehen auf A</t>
+  </si>
+  <si>
+    <t>mieć początek w [czymś], sięgać [czegoś]</t>
+  </si>
+  <si>
+    <t>staunen über A</t>
+  </si>
+  <si>
+    <t>dziwić się [komuś/czemuś]</t>
+  </si>
+  <si>
+    <t>sich widerspiegeln in D</t>
+  </si>
+  <si>
+    <t>odbijać/odzwierciedlać się w [czymś]</t>
+  </si>
+  <si>
+    <t>jdn aus-schließen aus D</t>
+  </si>
+  <si>
+    <t>usunąć, wykluczyć z [czegoś]</t>
+  </si>
+  <si>
+    <t>Zweifel haben an D</t>
+  </si>
+  <si>
+    <t>mieć wątpliwości co do [czegoś]</t>
+  </si>
+  <si>
+    <t>protestieren gegen A</t>
+  </si>
+  <si>
+    <t>protestować przeciwko [czemuś]</t>
+  </si>
+  <si>
+    <t>überreden zu D</t>
+  </si>
+  <si>
+    <t>namówić do [czegoś]</t>
+  </si>
+  <si>
+    <t>sich fernhalten von D</t>
+  </si>
+  <si>
+    <t>trzymać się z daleka od [kogoś/czegoś]</t>
+  </si>
+  <si>
+    <t>an-knüpfen an A</t>
+  </si>
+  <si>
+    <t>przywiązać do [czegoś]</t>
+  </si>
+  <si>
+    <t>basteln an D</t>
+  </si>
+  <si>
+    <t>majsterkować przy [czymś]</t>
+  </si>
+  <si>
+    <t>ein-steigen in A</t>
+  </si>
+  <si>
+    <t>wsiąść do [pojazdu]</t>
+  </si>
+  <si>
+    <t>hungrig sein auf A</t>
+  </si>
+  <si>
+    <t>mieć apetyt na [coś]</t>
+  </si>
+  <si>
+    <t>jdn ansprechen auf A</t>
+  </si>
+  <si>
+    <t>zwrócić się do kogoś w sprawie [czegoś]</t>
+  </si>
+  <si>
+    <t>kranken an D</t>
+  </si>
+  <si>
+    <t>chorować na [coś]</t>
+  </si>
+  <si>
+    <t>sich äußern zu D</t>
+  </si>
+  <si>
+    <t>wyrazić swoje zdanie co do [czegoś]</t>
+  </si>
+  <si>
+    <t>sich engagieren für A</t>
+  </si>
+  <si>
+    <t>zaangażować się [w]</t>
+  </si>
+  <si>
+    <t>sich erschrecken vor D</t>
+  </si>
+  <si>
+    <t>przestraszyć się [kogoś/czegoś]</t>
+  </si>
+  <si>
+    <t>sich zurechtfinden in D (z)</t>
+  </si>
+  <si>
+    <t>orientować się w [mieście/otoczeniu]</t>
+  </si>
+  <si>
+    <t>vorbei-schauen bei D</t>
+  </si>
+  <si>
+    <t>zaglądać, wstąpić do [kogoś]</t>
+  </si>
+  <si>
+    <t>verzweifeln an D</t>
+  </si>
+  <si>
+    <t>zwątpić w [coś]</t>
+  </si>
+  <si>
+    <t>vorbeireden an A</t>
+  </si>
+  <si>
+    <t>mówić o czymś innym niż rozmówca, nie rozumieć się</t>
+  </si>
+  <si>
+    <t>Anteil nehmen an D</t>
+  </si>
+  <si>
+    <t>wziąć w czymś udział</t>
+  </si>
+  <si>
+    <t>aus-rutschen auf D</t>
+  </si>
+  <si>
+    <t>poślizgnąć się na [czymś]</t>
+  </si>
+  <si>
+    <t>gut auskommen mit D</t>
+  </si>
+  <si>
+    <t>wytyrzymywać z [kimś]</t>
+  </si>
+  <si>
+    <t>jdm Bescheid geben über A</t>
+  </si>
+  <si>
+    <t>poinformować kogoś/dać komuś znać o [czymś]</t>
+  </si>
+  <si>
+    <t>sich bescheiden mit D</t>
+  </si>
+  <si>
+    <t>zadowolić się [czymś]</t>
+  </si>
+  <si>
+    <t>jdn überreden zu D</t>
+  </si>
+  <si>
+    <t>namówić/przekonać kogoś do [czegoś]</t>
+  </si>
+  <si>
+    <t>stolpern über A</t>
+  </si>
+  <si>
+    <t>potknąć się o [coś]</t>
+  </si>
+  <si>
+    <t>jdn unterstützen bei D</t>
+  </si>
+  <si>
+    <t>pomagać komuś/wspierać kogoś w [czymś]</t>
+  </si>
+  <si>
+    <t>sich verschanzen hinter D</t>
+  </si>
+  <si>
+    <t>ukrywać się za [czymś]</t>
+  </si>
+  <si>
+    <t>begeistert sein von D</t>
+  </si>
+  <si>
+    <t>być zachwyconym [czymś]</t>
   </si>
 </sst>
 </file>
@@ -1631,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:C253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="C214" sqref="C214"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="A214" sqref="A214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3354,6 +3582,310 @@
       </c>
       <c r="C214" t="s">
         <v>427</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" t="s">
+        <v>428</v>
+      </c>
+      <c r="C216" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" t="s">
+        <v>430</v>
+      </c>
+      <c r="C217" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" t="s">
+        <v>432</v>
+      </c>
+      <c r="C218" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" t="s">
+        <v>434</v>
+      </c>
+      <c r="C219" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" t="s">
+        <v>436</v>
+      </c>
+      <c r="C220" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" t="s">
+        <v>438</v>
+      </c>
+      <c r="C221" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" t="s">
+        <v>440</v>
+      </c>
+      <c r="C222" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" t="s">
+        <v>442</v>
+      </c>
+      <c r="C223" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" t="s">
+        <v>444</v>
+      </c>
+      <c r="C224" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" t="s">
+        <v>446</v>
+      </c>
+      <c r="C225" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" t="s">
+        <v>448</v>
+      </c>
+      <c r="C226" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" t="s">
+        <v>450</v>
+      </c>
+      <c r="C227" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" t="s">
+        <v>452</v>
+      </c>
+      <c r="C228" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" t="s">
+        <v>454</v>
+      </c>
+      <c r="C229" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" t="s">
+        <v>456</v>
+      </c>
+      <c r="C230" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" t="s">
+        <v>458</v>
+      </c>
+      <c r="C231" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" t="s">
+        <v>460</v>
+      </c>
+      <c r="C232" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" t="s">
+        <v>462</v>
+      </c>
+      <c r="C233" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" t="s">
+        <v>464</v>
+      </c>
+      <c r="C234" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" t="s">
+        <v>466</v>
+      </c>
+      <c r="C235" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" t="s">
+        <v>468</v>
+      </c>
+      <c r="C236" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237" t="s">
+        <v>470</v>
+      </c>
+      <c r="C237" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" t="s">
+        <v>472</v>
+      </c>
+      <c r="C238" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" t="s">
+        <v>474</v>
+      </c>
+      <c r="C239" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" t="s">
+        <v>476</v>
+      </c>
+      <c r="C240" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" t="s">
+        <v>478</v>
+      </c>
+      <c r="C241" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" t="s">
+        <v>480</v>
+      </c>
+      <c r="C242" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" t="s">
+        <v>482</v>
+      </c>
+      <c r="C243" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244" t="s">
+        <v>484</v>
+      </c>
+      <c r="C244" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245" t="s">
+        <v>486</v>
+      </c>
+      <c r="C245" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" t="s">
+        <v>488</v>
+      </c>
+      <c r="C246" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" t="s">
+        <v>490</v>
+      </c>
+      <c r="C247" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" t="s">
+        <v>492</v>
+      </c>
+      <c r="C248" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" t="s">
+        <v>494</v>
+      </c>
+      <c r="C249" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250" t="s">
+        <v>496</v>
+      </c>
+      <c r="C250" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251" t="s">
+        <v>498</v>
+      </c>
+      <c r="C251" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" t="s">
+        <v>500</v>
+      </c>
+      <c r="C252" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" t="s">
+        <v>502</v>
+      </c>
+      <c r="C253" t="s">
+        <v>503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>